<commit_message>
Minor change to test template
</commit_message>
<xml_diff>
--- a/Test_Template.xlsx
+++ b/Test_Template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aasav\github-classroom\EMAT31530\group-project-2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FC29D47-91B0-462E-8F33-D8BB508989AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1F680F5-5ACE-41D6-86B3-7F2715E286C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-86" yWindow="0" windowWidth="13029" windowHeight="16509" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="25920" windowHeight="16629" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="542" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="533" uniqueCount="106">
   <si>
     <t>Test ID</t>
   </si>
@@ -239,9 +239,6 @@
   </si>
   <si>
     <t>BEST OF ABOVE</t>
-  </si>
-  <si>
-    <t>Elitism selection, agents = 2</t>
   </si>
   <si>
     <t>""</t>
@@ -703,10 +700,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:X63"/>
+  <dimension ref="A1:X62"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Y24" sqref="Y24"/>
+      <selection activeCell="A37" sqref="A37:A62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -1980,10 +1977,10 @@
         <v>2</v>
       </c>
       <c r="J24" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="K24" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="L24" t="s">
         <v>26</v>
@@ -2033,10 +2030,10 @@
         <v>2</v>
       </c>
       <c r="J25" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="K25" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="L25" t="s">
         <v>26</v>
@@ -2086,10 +2083,10 @@
         <v>2</v>
       </c>
       <c r="J26" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="K26" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="L26" t="s">
         <v>26</v>
@@ -2139,10 +2136,10 @@
         <v>2</v>
       </c>
       <c r="J27" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="K27" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="L27" t="s">
         <v>26</v>
@@ -2192,10 +2189,10 @@
         <v>2</v>
       </c>
       <c r="J28" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="K28" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="L28" t="s">
         <v>26</v>
@@ -2245,10 +2242,10 @@
         <v>2</v>
       </c>
       <c r="J29" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="K29" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="L29" t="s">
         <v>26</v>
@@ -2298,10 +2295,10 @@
         <v>2</v>
       </c>
       <c r="J30" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="K30" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="L30" t="s">
         <v>26</v>
@@ -2351,10 +2348,10 @@
         <v>2</v>
       </c>
       <c r="J31" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="K31" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="L31" t="s">
         <v>26</v>
@@ -2404,10 +2401,10 @@
         <v>2</v>
       </c>
       <c r="J32" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="K32" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="L32" t="s">
         <v>26</v>
@@ -2457,10 +2454,10 @@
         <v>2</v>
       </c>
       <c r="J33" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="K33" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="L33" t="s">
         <v>26</v>
@@ -2510,10 +2507,10 @@
         <v>2</v>
       </c>
       <c r="J34" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="K34" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="L34" t="s">
         <v>26</v>
@@ -2563,10 +2560,10 @@
         <v>2</v>
       </c>
       <c r="J35" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="K35" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="L35" t="s">
         <v>26</v>
@@ -2616,10 +2613,10 @@
         <v>2</v>
       </c>
       <c r="J36" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="K36" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="L36" t="s">
         <v>26</v>
@@ -2669,10 +2666,10 @@
         <v>2</v>
       </c>
       <c r="J37" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="K37" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="L37" t="s">
         <v>26</v>
@@ -2719,31 +2716,31 @@
         <v>27</v>
       </c>
       <c r="I38">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="J38" t="s">
+        <v>73</v>
+      </c>
+      <c r="K38" t="s">
+        <v>73</v>
+      </c>
+      <c r="L38" t="s">
+        <v>26</v>
+      </c>
+      <c r="M38">
+        <v>0</v>
+      </c>
+      <c r="N38">
+        <v>0</v>
+      </c>
+      <c r="O38">
+        <v>0</v>
+      </c>
+      <c r="Q38">
+        <v>0</v>
+      </c>
+      <c r="S38" t="s">
         <v>74</v>
-      </c>
-      <c r="K38" t="s">
-        <v>74</v>
-      </c>
-      <c r="L38" t="s">
-        <v>26</v>
-      </c>
-      <c r="M38">
-        <v>0</v>
-      </c>
-      <c r="N38">
-        <v>0</v>
-      </c>
-      <c r="O38">
-        <v>0</v>
-      </c>
-      <c r="Q38">
-        <v>0</v>
-      </c>
-      <c r="S38" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="39" spans="1:19" x14ac:dyDescent="0.4">
@@ -2763,22 +2760,22 @@
         <v>25</v>
       </c>
       <c r="F39" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G39" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="H39" t="s">
         <v>27</v>
       </c>
       <c r="I39">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="J39" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="K39" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="L39" t="s">
         <v>26</v>
@@ -2816,22 +2813,22 @@
         <v>25</v>
       </c>
       <c r="F40" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G40" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="H40" t="s">
-        <v>27</v>
+        <v>76</v>
       </c>
       <c r="I40">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="J40" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="K40" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="L40" t="s">
         <v>26</v>
@@ -2849,7 +2846,7 @@
         <v>0</v>
       </c>
       <c r="S40" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="41" spans="1:19" x14ac:dyDescent="0.4">
@@ -2869,22 +2866,22 @@
         <v>25</v>
       </c>
       <c r="F41" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G41" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="H41" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="I41">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="J41" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="K41" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="L41" t="s">
         <v>26</v>
@@ -2922,22 +2919,22 @@
         <v>25</v>
       </c>
       <c r="F42" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G42" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="H42" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="I42">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="J42" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="K42" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="L42" t="s">
         <v>26</v>
@@ -2975,22 +2972,22 @@
         <v>25</v>
       </c>
       <c r="F43" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G43" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="H43" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="I43">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="J43" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="K43" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="L43" t="s">
         <v>26</v>
@@ -3008,7 +3005,7 @@
         <v>0</v>
       </c>
       <c r="S43" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="44" spans="1:19" x14ac:dyDescent="0.4">
@@ -3028,22 +3025,22 @@
         <v>25</v>
       </c>
       <c r="F44" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G44" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="H44" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I44">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="J44" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="K44" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="L44" t="s">
         <v>26</v>
@@ -3081,22 +3078,22 @@
         <v>25</v>
       </c>
       <c r="F45" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G45" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="H45" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I45">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="J45" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="K45" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="L45" t="s">
         <v>26</v>
@@ -3134,22 +3131,22 @@
         <v>25</v>
       </c>
       <c r="F46" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G46" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="H46" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="I46">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="J46" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="K46" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="L46" t="s">
         <v>26</v>
@@ -3167,7 +3164,7 @@
         <v>0</v>
       </c>
       <c r="S46" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="47" spans="1:19" x14ac:dyDescent="0.4">
@@ -3187,22 +3184,22 @@
         <v>25</v>
       </c>
       <c r="F47" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G47" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="H47" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="I47">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="J47" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="K47" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="L47" t="s">
         <v>26</v>
@@ -3240,22 +3237,22 @@
         <v>25</v>
       </c>
       <c r="F48" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G48" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="H48" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="I48">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="J48" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="K48" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="L48" t="s">
         <v>26</v>
@@ -3293,28 +3290,28 @@
         <v>25</v>
       </c>
       <c r="F49" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G49" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="H49" t="s">
-        <v>85</v>
-      </c>
-      <c r="I49">
-        <v>10</v>
+        <v>72</v>
+      </c>
+      <c r="I49" t="s">
+        <v>72</v>
       </c>
       <c r="J49" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="K49" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="L49" t="s">
-        <v>26</v>
+        <v>88</v>
       </c>
       <c r="M49">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="N49">
         <v>0</v>
@@ -3326,7 +3323,7 @@
         <v>0</v>
       </c>
       <c r="S49" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="50" spans="1:19" x14ac:dyDescent="0.4">
@@ -3346,28 +3343,28 @@
         <v>25</v>
       </c>
       <c r="F50" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G50" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="H50" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="I50" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="J50" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="K50" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="L50" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="M50">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="N50">
         <v>0</v>
@@ -3399,28 +3396,28 @@
         <v>25</v>
       </c>
       <c r="F51" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G51" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="H51" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I51" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="J51" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="K51" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="L51" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="M51">
-        <v>0.2</v>
+        <v>0.5</v>
       </c>
       <c r="N51">
         <v>0</v>
@@ -3452,28 +3449,28 @@
         <v>25</v>
       </c>
       <c r="F52" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G52" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="H52" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I52" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="J52" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="K52" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="L52" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="M52">
-        <v>0.5</v>
+        <v>0.1</v>
       </c>
       <c r="N52">
         <v>0</v>
@@ -3485,7 +3482,7 @@
         <v>0</v>
       </c>
       <c r="S52" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
     </row>
     <row r="53" spans="1:19" x14ac:dyDescent="0.4">
@@ -3505,28 +3502,28 @@
         <v>25</v>
       </c>
       <c r="F53" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G53" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="H53" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I53" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="J53" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="K53" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="L53" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="M53">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="N53">
         <v>0</v>
@@ -3558,28 +3555,28 @@
         <v>25</v>
       </c>
       <c r="F54" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G54" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="H54" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I54" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="J54" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="K54" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="L54" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="M54">
-        <v>0.2</v>
+        <v>0.5</v>
       </c>
       <c r="N54">
         <v>0</v>
@@ -3611,28 +3608,28 @@
         <v>25</v>
       </c>
       <c r="F55" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G55" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="H55" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I55" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="J55" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="K55" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="L55" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="M55">
-        <v>0.5</v>
+        <v>0.1</v>
       </c>
       <c r="N55">
         <v>0</v>
@@ -3644,7 +3641,7 @@
         <v>0</v>
       </c>
       <c r="S55" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
     </row>
     <row r="56" spans="1:19" x14ac:dyDescent="0.4">
@@ -3664,28 +3661,28 @@
         <v>25</v>
       </c>
       <c r="F56" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G56" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="H56" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I56" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="J56" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="K56" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="L56" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="M56">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="N56">
         <v>0</v>
@@ -3717,28 +3714,28 @@
         <v>25</v>
       </c>
       <c r="F57" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G57" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="H57" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I57" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="J57" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="K57" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="L57" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="M57">
-        <v>0.2</v>
+        <v>0.5</v>
       </c>
       <c r="N57">
         <v>0</v>
@@ -3770,28 +3767,28 @@
         <v>25</v>
       </c>
       <c r="F58" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G58" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="H58" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I58" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="J58" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="K58" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="L58" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="M58">
-        <v>0.5</v>
+        <v>0.1</v>
       </c>
       <c r="N58">
         <v>0</v>
@@ -3803,7 +3800,7 @@
         <v>0</v>
       </c>
       <c r="S58" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
     </row>
     <row r="59" spans="1:19" x14ac:dyDescent="0.4">
@@ -3823,28 +3820,28 @@
         <v>25</v>
       </c>
       <c r="F59" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G59" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="H59" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I59" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="J59" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="K59" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="L59" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="M59">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="N59">
         <v>0</v>
@@ -3876,28 +3873,28 @@
         <v>25</v>
       </c>
       <c r="F60" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G60" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="H60" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I60" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="J60" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="K60" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="L60" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="M60">
-        <v>0.2</v>
+        <v>0.5</v>
       </c>
       <c r="N60">
         <v>0</v>
@@ -3929,31 +3926,31 @@
         <v>25</v>
       </c>
       <c r="F61" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G61" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="H61" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I61" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="J61" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="K61" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="L61" t="s">
-        <v>101</v>
-      </c>
-      <c r="M61">
-        <v>0.5</v>
+        <v>72</v>
+      </c>
+      <c r="M61" t="s">
+        <v>72</v>
       </c>
       <c r="N61">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O61">
         <v>0</v>
@@ -3982,93 +3979,40 @@
         <v>25</v>
       </c>
       <c r="F62" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G62" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="H62" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I62" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="J62" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="K62" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="L62" t="s">
+        <v>73</v>
+      </c>
+      <c r="M62" t="s">
+        <v>73</v>
+      </c>
+      <c r="N62" t="s">
         <v>72</v>
       </c>
-      <c r="M62" t="s">
-        <v>72</v>
-      </c>
-      <c r="N62">
+      <c r="O62">
         <v>1</v>
-      </c>
-      <c r="O62">
-        <v>0</v>
       </c>
       <c r="Q62">
         <v>0</v>
       </c>
       <c r="S62" t="s">
         <v>105</v>
-      </c>
-    </row>
-    <row r="63" spans="1:19" x14ac:dyDescent="0.4">
-      <c r="A63">
-        <v>61</v>
-      </c>
-      <c r="B63" t="s">
-        <v>24</v>
-      </c>
-      <c r="C63">
-        <v>20</v>
-      </c>
-      <c r="D63">
-        <v>20</v>
-      </c>
-      <c r="E63" t="s">
-        <v>25</v>
-      </c>
-      <c r="F63" t="s">
-        <v>74</v>
-      </c>
-      <c r="G63" t="s">
-        <v>74</v>
-      </c>
-      <c r="H63" t="s">
-        <v>74</v>
-      </c>
-      <c r="I63" t="s">
-        <v>74</v>
-      </c>
-      <c r="J63" t="s">
-        <v>74</v>
-      </c>
-      <c r="K63" t="s">
-        <v>74</v>
-      </c>
-      <c r="L63" t="s">
-        <v>74</v>
-      </c>
-      <c r="M63" t="s">
-        <v>74</v>
-      </c>
-      <c r="N63" t="s">
-        <v>72</v>
-      </c>
-      <c r="O63">
-        <v>1</v>
-      </c>
-      <c r="Q63">
-        <v>0</v>
-      </c>
-      <c r="S63" t="s">
-        <v>106</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changed the order of tests
</commit_message>
<xml_diff>
--- a/Test_Template.xlsx
+++ b/Test_Template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aasav\github-classroom\EMAT31530\group-project-2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1F680F5-5ACE-41D6-86B3-7F2715E286C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A274D455-0D48-4E06-85C8-16F69B340EE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="25920" windowHeight="16629" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="533" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="553" uniqueCount="106">
   <si>
     <t>Test ID</t>
   </si>
@@ -703,7 +703,7 @@
   <dimension ref="A1:X62"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A37" sqref="A37:A62"/>
+      <selection activeCell="V50" sqref="V50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -829,7 +829,7 @@
         <v>0</v>
       </c>
       <c r="Q2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S2" t="s">
         <v>28</v>
@@ -882,7 +882,7 @@
         <v>0</v>
       </c>
       <c r="Q3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S3" t="s">
         <v>29</v>
@@ -935,7 +935,7 @@
         <v>0</v>
       </c>
       <c r="Q4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S4" t="s">
         <v>30</v>
@@ -988,7 +988,7 @@
         <v>0</v>
       </c>
       <c r="Q5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S5" t="s">
         <v>31</v>
@@ -1041,7 +1041,7 @@
         <v>0</v>
       </c>
       <c r="Q6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S6" t="s">
         <v>32</v>
@@ -1073,13 +1073,13 @@
         <v>27</v>
       </c>
       <c r="I7">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="J7" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="K7">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="L7" t="s">
         <v>26</v>
@@ -1094,10 +1094,10 @@
         <v>0</v>
       </c>
       <c r="Q7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S7" t="s">
-        <v>34</v>
+        <v>74</v>
       </c>
     </row>
     <row r="8" spans="1:24" x14ac:dyDescent="0.4">
@@ -1126,13 +1126,13 @@
         <v>27</v>
       </c>
       <c r="I8">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="J8" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="K8">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="L8" t="s">
         <v>26</v>
@@ -1147,10 +1147,10 @@
         <v>0</v>
       </c>
       <c r="Q8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S8" t="s">
-        <v>35</v>
+        <v>75</v>
       </c>
     </row>
     <row r="9" spans="1:24" x14ac:dyDescent="0.4">
@@ -1176,16 +1176,16 @@
         <v>0</v>
       </c>
       <c r="H9" t="s">
-        <v>27</v>
+        <v>76</v>
       </c>
       <c r="I9">
         <v>2</v>
       </c>
       <c r="J9" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="K9">
-        <v>0.7</v>
+        <v>0</v>
       </c>
       <c r="L9" t="s">
         <v>26</v>
@@ -1200,10 +1200,10 @@
         <v>0</v>
       </c>
       <c r="Q9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S9" t="s">
-        <v>36</v>
+        <v>77</v>
       </c>
     </row>
     <row r="10" spans="1:24" x14ac:dyDescent="0.4">
@@ -1229,16 +1229,16 @@
         <v>0</v>
       </c>
       <c r="H10" t="s">
-        <v>27</v>
+        <v>76</v>
       </c>
       <c r="I10">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="J10" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="K10">
-        <v>0.9</v>
+        <v>0</v>
       </c>
       <c r="L10" t="s">
         <v>26</v>
@@ -1253,10 +1253,10 @@
         <v>0</v>
       </c>
       <c r="Q10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S10" t="s">
-        <v>37</v>
+        <v>78</v>
       </c>
     </row>
     <row r="11" spans="1:24" x14ac:dyDescent="0.4">
@@ -1282,16 +1282,16 @@
         <v>0</v>
       </c>
       <c r="H11" t="s">
-        <v>27</v>
+        <v>76</v>
       </c>
       <c r="I11">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="J11" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="K11">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="L11" t="s">
         <v>26</v>
@@ -1306,10 +1306,10 @@
         <v>0</v>
       </c>
       <c r="Q11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S11" t="s">
-        <v>39</v>
+        <v>79</v>
       </c>
     </row>
     <row r="12" spans="1:24" x14ac:dyDescent="0.4">
@@ -1335,16 +1335,16 @@
         <v>0</v>
       </c>
       <c r="H12" t="s">
-        <v>27</v>
+        <v>80</v>
       </c>
       <c r="I12">
         <v>2</v>
       </c>
       <c r="J12" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="K12">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="L12" t="s">
         <v>26</v>
@@ -1359,10 +1359,10 @@
         <v>0</v>
       </c>
       <c r="Q12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S12" t="s">
-        <v>40</v>
+        <v>81</v>
       </c>
     </row>
     <row r="13" spans="1:24" x14ac:dyDescent="0.4">
@@ -1388,16 +1388,16 @@
         <v>0</v>
       </c>
       <c r="H13" t="s">
-        <v>27</v>
+        <v>80</v>
       </c>
       <c r="I13">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="J13" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="K13">
-        <v>0.7</v>
+        <v>0</v>
       </c>
       <c r="L13" t="s">
         <v>26</v>
@@ -1412,10 +1412,10 @@
         <v>0</v>
       </c>
       <c r="Q13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S13" t="s">
-        <v>41</v>
+        <v>82</v>
       </c>
     </row>
     <row r="14" spans="1:24" x14ac:dyDescent="0.4">
@@ -1441,16 +1441,16 @@
         <v>0</v>
       </c>
       <c r="H14" t="s">
-        <v>27</v>
+        <v>80</v>
       </c>
       <c r="I14">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="J14" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="K14">
-        <v>0.9</v>
+        <v>0</v>
       </c>
       <c r="L14" t="s">
         <v>26</v>
@@ -1465,10 +1465,10 @@
         <v>0</v>
       </c>
       <c r="Q14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S14" t="s">
-        <v>42</v>
+        <v>83</v>
       </c>
     </row>
     <row r="15" spans="1:24" x14ac:dyDescent="0.4">
@@ -1494,16 +1494,16 @@
         <v>0</v>
       </c>
       <c r="H15" t="s">
-        <v>27</v>
+        <v>84</v>
       </c>
       <c r="I15">
         <v>2</v>
       </c>
       <c r="J15" t="s">
-        <v>43</v>
+        <v>26</v>
       </c>
       <c r="K15">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="L15" t="s">
         <v>26</v>
@@ -1518,10 +1518,10 @@
         <v>0</v>
       </c>
       <c r="Q15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S15" t="s">
-        <v>44</v>
+        <v>85</v>
       </c>
     </row>
     <row r="16" spans="1:24" x14ac:dyDescent="0.4">
@@ -1547,16 +1547,16 @@
         <v>0</v>
       </c>
       <c r="H16" t="s">
-        <v>27</v>
+        <v>84</v>
       </c>
       <c r="I16">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="J16" t="s">
-        <v>43</v>
+        <v>26</v>
       </c>
       <c r="K16">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="L16" t="s">
         <v>26</v>
@@ -1571,10 +1571,10 @@
         <v>0</v>
       </c>
       <c r="Q16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S16" t="s">
-        <v>45</v>
+        <v>86</v>
       </c>
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.4">
@@ -1600,16 +1600,16 @@
         <v>0</v>
       </c>
       <c r="H17" t="s">
-        <v>27</v>
+        <v>84</v>
       </c>
       <c r="I17">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="J17" t="s">
-        <v>43</v>
+        <v>26</v>
       </c>
       <c r="K17">
-        <v>0.7</v>
+        <v>0</v>
       </c>
       <c r="L17" t="s">
         <v>26</v>
@@ -1624,10 +1624,10 @@
         <v>0</v>
       </c>
       <c r="Q17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S17" t="s">
-        <v>46</v>
+        <v>87</v>
       </c>
     </row>
     <row r="18" spans="1:19" x14ac:dyDescent="0.4">
@@ -1653,16 +1653,16 @@
         <v>0</v>
       </c>
       <c r="H18" t="s">
-        <v>27</v>
-      </c>
-      <c r="I18">
-        <v>2</v>
+        <v>72</v>
+      </c>
+      <c r="I18" t="s">
+        <v>72</v>
       </c>
       <c r="J18" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="K18">
-        <v>0.9</v>
+        <v>0.2</v>
       </c>
       <c r="L18" t="s">
         <v>26</v>
@@ -1677,10 +1677,10 @@
         <v>0</v>
       </c>
       <c r="Q18">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S18" t="s">
-        <v>47</v>
+        <v>34</v>
       </c>
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.4">
@@ -1706,16 +1706,16 @@
         <v>0</v>
       </c>
       <c r="H19" t="s">
-        <v>27</v>
-      </c>
-      <c r="I19">
-        <v>2</v>
+        <v>73</v>
+      </c>
+      <c r="I19" t="s">
+        <v>73</v>
       </c>
       <c r="J19" t="s">
-        <v>48</v>
+        <v>33</v>
       </c>
       <c r="K19">
-        <v>0.2</v>
+        <v>0.5</v>
       </c>
       <c r="L19" t="s">
         <v>26</v>
@@ -1730,10 +1730,10 @@
         <v>0</v>
       </c>
       <c r="Q19">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S19" t="s">
-        <v>49</v>
+        <v>35</v>
       </c>
     </row>
     <row r="20" spans="1:19" x14ac:dyDescent="0.4">
@@ -1759,16 +1759,16 @@
         <v>0</v>
       </c>
       <c r="H20" t="s">
-        <v>27</v>
-      </c>
-      <c r="I20">
-        <v>2</v>
+        <v>73</v>
+      </c>
+      <c r="I20" t="s">
+        <v>73</v>
       </c>
       <c r="J20" t="s">
-        <v>48</v>
+        <v>33</v>
       </c>
       <c r="K20">
-        <v>0.5</v>
+        <v>0.7</v>
       </c>
       <c r="L20" t="s">
         <v>26</v>
@@ -1783,10 +1783,10 @@
         <v>0</v>
       </c>
       <c r="Q20">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S20" t="s">
-        <v>50</v>
+        <v>36</v>
       </c>
     </row>
     <row r="21" spans="1:19" x14ac:dyDescent="0.4">
@@ -1812,16 +1812,16 @@
         <v>0</v>
       </c>
       <c r="H21" t="s">
-        <v>27</v>
-      </c>
-      <c r="I21">
-        <v>2</v>
+        <v>73</v>
+      </c>
+      <c r="I21" t="s">
+        <v>73</v>
       </c>
       <c r="J21" t="s">
-        <v>48</v>
+        <v>33</v>
       </c>
       <c r="K21">
-        <v>0.7</v>
+        <v>0.9</v>
       </c>
       <c r="L21" t="s">
         <v>26</v>
@@ -1836,10 +1836,10 @@
         <v>0</v>
       </c>
       <c r="Q21">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S21" t="s">
-        <v>51</v>
+        <v>37</v>
       </c>
     </row>
     <row r="22" spans="1:19" x14ac:dyDescent="0.4">
@@ -1865,16 +1865,16 @@
         <v>0</v>
       </c>
       <c r="H22" t="s">
-        <v>27</v>
-      </c>
-      <c r="I22">
-        <v>2</v>
+        <v>73</v>
+      </c>
+      <c r="I22" t="s">
+        <v>73</v>
       </c>
       <c r="J22" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="K22">
-        <v>0.9</v>
+        <v>0.2</v>
       </c>
       <c r="L22" t="s">
         <v>26</v>
@@ -1889,10 +1889,10 @@
         <v>0</v>
       </c>
       <c r="Q22">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S22" t="s">
-        <v>52</v>
+        <v>39</v>
       </c>
     </row>
     <row r="23" spans="1:19" x14ac:dyDescent="0.4">
@@ -1912,22 +1912,22 @@
         <v>25</v>
       </c>
       <c r="F23" t="s">
-        <v>53</v>
+        <v>26</v>
       </c>
       <c r="G23">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="H23" t="s">
-        <v>27</v>
-      </c>
-      <c r="I23">
-        <v>2</v>
+        <v>73</v>
+      </c>
+      <c r="I23" t="s">
+        <v>73</v>
       </c>
       <c r="J23" t="s">
-        <v>72</v>
-      </c>
-      <c r="K23" t="s">
-        <v>72</v>
+        <v>38</v>
+      </c>
+      <c r="K23">
+        <v>0.5</v>
       </c>
       <c r="L23" t="s">
         <v>26</v>
@@ -1942,10 +1942,10 @@
         <v>0</v>
       </c>
       <c r="Q23">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S23" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
     </row>
     <row r="24" spans="1:19" x14ac:dyDescent="0.4">
@@ -1965,22 +1965,22 @@
         <v>25</v>
       </c>
       <c r="F24" t="s">
-        <v>53</v>
+        <v>26</v>
       </c>
       <c r="G24">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="H24" t="s">
-        <v>27</v>
-      </c>
-      <c r="I24">
-        <v>2</v>
+        <v>73</v>
+      </c>
+      <c r="I24" t="s">
+        <v>73</v>
       </c>
       <c r="J24" t="s">
-        <v>73</v>
-      </c>
-      <c r="K24" t="s">
-        <v>73</v>
+        <v>38</v>
+      </c>
+      <c r="K24">
+        <v>0.7</v>
       </c>
       <c r="L24" t="s">
         <v>26</v>
@@ -1995,10 +1995,10 @@
         <v>0</v>
       </c>
       <c r="Q24">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S24" t="s">
-        <v>55</v>
+        <v>41</v>
       </c>
     </row>
     <row r="25" spans="1:19" x14ac:dyDescent="0.4">
@@ -2018,22 +2018,22 @@
         <v>25</v>
       </c>
       <c r="F25" t="s">
-        <v>53</v>
+        <v>26</v>
       </c>
       <c r="G25">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="H25" t="s">
-        <v>27</v>
-      </c>
-      <c r="I25">
-        <v>2</v>
+        <v>73</v>
+      </c>
+      <c r="I25" t="s">
+        <v>73</v>
       </c>
       <c r="J25" t="s">
-        <v>73</v>
-      </c>
-      <c r="K25" t="s">
-        <v>73</v>
+        <v>38</v>
+      </c>
+      <c r="K25">
+        <v>0.9</v>
       </c>
       <c r="L25" t="s">
         <v>26</v>
@@ -2048,10 +2048,10 @@
         <v>0</v>
       </c>
       <c r="Q25">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S25" t="s">
-        <v>56</v>
+        <v>42</v>
       </c>
     </row>
     <row r="26" spans="1:19" x14ac:dyDescent="0.4">
@@ -2071,22 +2071,22 @@
         <v>25</v>
       </c>
       <c r="F26" t="s">
-        <v>57</v>
+        <v>26</v>
       </c>
       <c r="G26">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="H26" t="s">
-        <v>27</v>
-      </c>
-      <c r="I26">
-        <v>2</v>
+        <v>73</v>
+      </c>
+      <c r="I26" t="s">
+        <v>73</v>
       </c>
       <c r="J26" t="s">
-        <v>73</v>
-      </c>
-      <c r="K26" t="s">
-        <v>73</v>
+        <v>43</v>
+      </c>
+      <c r="K26">
+        <v>0.2</v>
       </c>
       <c r="L26" t="s">
         <v>26</v>
@@ -2101,10 +2101,10 @@
         <v>0</v>
       </c>
       <c r="Q26">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S26" t="s">
-        <v>58</v>
+        <v>44</v>
       </c>
     </row>
     <row r="27" spans="1:19" x14ac:dyDescent="0.4">
@@ -2124,22 +2124,22 @@
         <v>25</v>
       </c>
       <c r="F27" t="s">
-        <v>57</v>
+        <v>26</v>
       </c>
       <c r="G27">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="H27" t="s">
-        <v>27</v>
-      </c>
-      <c r="I27">
-        <v>2</v>
+        <v>73</v>
+      </c>
+      <c r="I27" t="s">
+        <v>73</v>
       </c>
       <c r="J27" t="s">
-        <v>73</v>
-      </c>
-      <c r="K27" t="s">
-        <v>73</v>
+        <v>43</v>
+      </c>
+      <c r="K27">
+        <v>0.5</v>
       </c>
       <c r="L27" t="s">
         <v>26</v>
@@ -2154,10 +2154,10 @@
         <v>0</v>
       </c>
       <c r="Q27">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S27" t="s">
-        <v>59</v>
+        <v>45</v>
       </c>
     </row>
     <row r="28" spans="1:19" x14ac:dyDescent="0.4">
@@ -2177,22 +2177,22 @@
         <v>25</v>
       </c>
       <c r="F28" t="s">
-        <v>57</v>
+        <v>26</v>
       </c>
       <c r="G28">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="H28" t="s">
-        <v>27</v>
-      </c>
-      <c r="I28">
-        <v>2</v>
+        <v>73</v>
+      </c>
+      <c r="I28" t="s">
+        <v>73</v>
       </c>
       <c r="J28" t="s">
-        <v>73</v>
-      </c>
-      <c r="K28" t="s">
-        <v>73</v>
+        <v>43</v>
+      </c>
+      <c r="K28">
+        <v>0.7</v>
       </c>
       <c r="L28" t="s">
         <v>26</v>
@@ -2207,10 +2207,10 @@
         <v>0</v>
       </c>
       <c r="Q28">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S28" t="s">
-        <v>60</v>
+        <v>46</v>
       </c>
     </row>
     <row r="29" spans="1:19" x14ac:dyDescent="0.4">
@@ -2230,22 +2230,22 @@
         <v>25</v>
       </c>
       <c r="F29" t="s">
-        <v>61</v>
+        <v>26</v>
       </c>
       <c r="G29">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="H29" t="s">
-        <v>27</v>
-      </c>
-      <c r="I29">
-        <v>2</v>
+        <v>73</v>
+      </c>
+      <c r="I29" t="s">
+        <v>73</v>
       </c>
       <c r="J29" t="s">
-        <v>73</v>
-      </c>
-      <c r="K29" t="s">
-        <v>73</v>
+        <v>43</v>
+      </c>
+      <c r="K29">
+        <v>0.9</v>
       </c>
       <c r="L29" t="s">
         <v>26</v>
@@ -2260,10 +2260,10 @@
         <v>0</v>
       </c>
       <c r="Q29">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S29" t="s">
-        <v>62</v>
+        <v>47</v>
       </c>
     </row>
     <row r="30" spans="1:19" x14ac:dyDescent="0.4">
@@ -2283,23 +2283,23 @@
         <v>25</v>
       </c>
       <c r="F30" t="s">
-        <v>61</v>
+        <v>26</v>
       </c>
       <c r="G30">
+        <v>0</v>
+      </c>
+      <c r="H30" t="s">
+        <v>73</v>
+      </c>
+      <c r="I30" t="s">
+        <v>73</v>
+      </c>
+      <c r="J30" t="s">
+        <v>48</v>
+      </c>
+      <c r="K30">
         <v>0.2</v>
       </c>
-      <c r="H30" t="s">
-        <v>27</v>
-      </c>
-      <c r="I30">
-        <v>2</v>
-      </c>
-      <c r="J30" t="s">
-        <v>73</v>
-      </c>
-      <c r="K30" t="s">
-        <v>73</v>
-      </c>
       <c r="L30" t="s">
         <v>26</v>
       </c>
@@ -2313,10 +2313,10 @@
         <v>0</v>
       </c>
       <c r="Q30">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S30" t="s">
-        <v>63</v>
+        <v>49</v>
       </c>
     </row>
     <row r="31" spans="1:19" x14ac:dyDescent="0.4">
@@ -2336,23 +2336,23 @@
         <v>25</v>
       </c>
       <c r="F31" t="s">
-        <v>61</v>
+        <v>26</v>
       </c>
       <c r="G31">
+        <v>0</v>
+      </c>
+      <c r="H31" t="s">
+        <v>73</v>
+      </c>
+      <c r="I31" t="s">
+        <v>73</v>
+      </c>
+      <c r="J31" t="s">
+        <v>48</v>
+      </c>
+      <c r="K31">
         <v>0.5</v>
       </c>
-      <c r="H31" t="s">
-        <v>27</v>
-      </c>
-      <c r="I31">
-        <v>2</v>
-      </c>
-      <c r="J31" t="s">
-        <v>73</v>
-      </c>
-      <c r="K31" t="s">
-        <v>73</v>
-      </c>
       <c r="L31" t="s">
         <v>26</v>
       </c>
@@ -2366,10 +2366,10 @@
         <v>0</v>
       </c>
       <c r="Q31">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S31" t="s">
-        <v>64</v>
+        <v>50</v>
       </c>
     </row>
     <row r="32" spans="1:19" x14ac:dyDescent="0.4">
@@ -2389,22 +2389,22 @@
         <v>25</v>
       </c>
       <c r="F32" t="s">
-        <v>65</v>
+        <v>26</v>
       </c>
       <c r="G32">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="H32" t="s">
-        <v>27</v>
-      </c>
-      <c r="I32">
-        <v>2</v>
+        <v>73</v>
+      </c>
+      <c r="I32" t="s">
+        <v>73</v>
       </c>
       <c r="J32" t="s">
-        <v>73</v>
-      </c>
-      <c r="K32" t="s">
-        <v>73</v>
+        <v>48</v>
+      </c>
+      <c r="K32">
+        <v>0.7</v>
       </c>
       <c r="L32" t="s">
         <v>26</v>
@@ -2419,10 +2419,10 @@
         <v>0</v>
       </c>
       <c r="Q32">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S32" t="s">
-        <v>66</v>
+        <v>51</v>
       </c>
     </row>
     <row r="33" spans="1:19" x14ac:dyDescent="0.4">
@@ -2442,22 +2442,22 @@
         <v>25</v>
       </c>
       <c r="F33" t="s">
-        <v>65</v>
+        <v>26</v>
       </c>
       <c r="G33">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="H33" t="s">
-        <v>27</v>
-      </c>
-      <c r="I33">
-        <v>2</v>
+        <v>73</v>
+      </c>
+      <c r="I33" t="s">
+        <v>73</v>
       </c>
       <c r="J33" t="s">
-        <v>73</v>
-      </c>
-      <c r="K33" t="s">
-        <v>73</v>
+        <v>48</v>
+      </c>
+      <c r="K33">
+        <v>0.9</v>
       </c>
       <c r="L33" t="s">
         <v>26</v>
@@ -2472,10 +2472,10 @@
         <v>0</v>
       </c>
       <c r="Q33">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S33" t="s">
-        <v>67</v>
+        <v>52</v>
       </c>
     </row>
     <row r="34" spans="1:19" x14ac:dyDescent="0.4">
@@ -2495,22 +2495,22 @@
         <v>25</v>
       </c>
       <c r="F34" t="s">
-        <v>65</v>
+        <v>53</v>
       </c>
       <c r="G34">
-        <v>0.5</v>
+        <v>0.1</v>
       </c>
       <c r="H34" t="s">
-        <v>27</v>
-      </c>
-      <c r="I34">
-        <v>2</v>
+        <v>73</v>
+      </c>
+      <c r="I34" t="s">
+        <v>73</v>
       </c>
       <c r="J34" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="K34" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="L34" t="s">
         <v>26</v>
@@ -2525,10 +2525,10 @@
         <v>0</v>
       </c>
       <c r="Q34">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S34" t="s">
-        <v>68</v>
+        <v>54</v>
       </c>
     </row>
     <row r="35" spans="1:19" x14ac:dyDescent="0.4">
@@ -2548,16 +2548,16 @@
         <v>25</v>
       </c>
       <c r="F35" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="G35">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="H35" t="s">
-        <v>27</v>
-      </c>
-      <c r="I35">
-        <v>2</v>
+        <v>73</v>
+      </c>
+      <c r="I35" t="s">
+        <v>73</v>
       </c>
       <c r="J35" t="s">
         <v>73</v>
@@ -2578,10 +2578,10 @@
         <v>0</v>
       </c>
       <c r="Q35">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S35" t="s">
-        <v>69</v>
+        <v>55</v>
       </c>
     </row>
     <row r="36" spans="1:19" x14ac:dyDescent="0.4">
@@ -2601,16 +2601,16 @@
         <v>25</v>
       </c>
       <c r="F36" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="G36">
-        <v>0.2</v>
+        <v>0.5</v>
       </c>
       <c r="H36" t="s">
-        <v>27</v>
-      </c>
-      <c r="I36">
-        <v>2</v>
+        <v>73</v>
+      </c>
+      <c r="I36" t="s">
+        <v>73</v>
       </c>
       <c r="J36" t="s">
         <v>73</v>
@@ -2631,10 +2631,10 @@
         <v>0</v>
       </c>
       <c r="Q36">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S36" t="s">
-        <v>70</v>
+        <v>56</v>
       </c>
     </row>
     <row r="37" spans="1:19" x14ac:dyDescent="0.4">
@@ -2654,16 +2654,16 @@
         <v>25</v>
       </c>
       <c r="F37" t="s">
-        <v>48</v>
+        <v>57</v>
       </c>
       <c r="G37">
-        <v>0.5</v>
+        <v>0.1</v>
       </c>
       <c r="H37" t="s">
-        <v>27</v>
-      </c>
-      <c r="I37">
-        <v>2</v>
+        <v>73</v>
+      </c>
+      <c r="I37" t="s">
+        <v>73</v>
       </c>
       <c r="J37" t="s">
         <v>73</v>
@@ -2684,10 +2684,10 @@
         <v>0</v>
       </c>
       <c r="Q37">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S37" t="s">
-        <v>71</v>
+        <v>58</v>
       </c>
     </row>
     <row r="38" spans="1:19" x14ac:dyDescent="0.4">
@@ -2707,16 +2707,16 @@
         <v>25</v>
       </c>
       <c r="F38" t="s">
-        <v>72</v>
-      </c>
-      <c r="G38" t="s">
-        <v>72</v>
+        <v>57</v>
+      </c>
+      <c r="G38">
+        <v>0.2</v>
       </c>
       <c r="H38" t="s">
-        <v>27</v>
-      </c>
-      <c r="I38">
-        <v>5</v>
+        <v>73</v>
+      </c>
+      <c r="I38" t="s">
+        <v>73</v>
       </c>
       <c r="J38" t="s">
         <v>73</v>
@@ -2740,7 +2740,7 @@
         <v>0</v>
       </c>
       <c r="S38" t="s">
-        <v>74</v>
+        <v>59</v>
       </c>
     </row>
     <row r="39" spans="1:19" x14ac:dyDescent="0.4">
@@ -2760,16 +2760,16 @@
         <v>25</v>
       </c>
       <c r="F39" t="s">
-        <v>73</v>
-      </c>
-      <c r="G39" t="s">
-        <v>73</v>
+        <v>57</v>
+      </c>
+      <c r="G39">
+        <v>0.5</v>
       </c>
       <c r="H39" t="s">
-        <v>27</v>
-      </c>
-      <c r="I39">
-        <v>10</v>
+        <v>73</v>
+      </c>
+      <c r="I39" t="s">
+        <v>73</v>
       </c>
       <c r="J39" t="s">
         <v>73</v>
@@ -2793,7 +2793,7 @@
         <v>0</v>
       </c>
       <c r="S39" t="s">
-        <v>75</v>
+        <v>60</v>
       </c>
     </row>
     <row r="40" spans="1:19" x14ac:dyDescent="0.4">
@@ -2813,16 +2813,16 @@
         <v>25</v>
       </c>
       <c r="F40" t="s">
-        <v>73</v>
-      </c>
-      <c r="G40" t="s">
-        <v>73</v>
+        <v>61</v>
+      </c>
+      <c r="G40">
+        <v>0.1</v>
       </c>
       <c r="H40" t="s">
-        <v>76</v>
-      </c>
-      <c r="I40">
-        <v>2</v>
+        <v>73</v>
+      </c>
+      <c r="I40" t="s">
+        <v>73</v>
       </c>
       <c r="J40" t="s">
         <v>73</v>
@@ -2846,7 +2846,7 @@
         <v>0</v>
       </c>
       <c r="S40" t="s">
-        <v>77</v>
+        <v>62</v>
       </c>
     </row>
     <row r="41" spans="1:19" x14ac:dyDescent="0.4">
@@ -2866,16 +2866,16 @@
         <v>25</v>
       </c>
       <c r="F41" t="s">
-        <v>73</v>
-      </c>
-      <c r="G41" t="s">
-        <v>73</v>
+        <v>61</v>
+      </c>
+      <c r="G41">
+        <v>0.2</v>
       </c>
       <c r="H41" t="s">
-        <v>76</v>
-      </c>
-      <c r="I41">
-        <v>5</v>
+        <v>73</v>
+      </c>
+      <c r="I41" t="s">
+        <v>73</v>
       </c>
       <c r="J41" t="s">
         <v>73</v>
@@ -2899,7 +2899,7 @@
         <v>0</v>
       </c>
       <c r="S41" t="s">
-        <v>78</v>
+        <v>63</v>
       </c>
     </row>
     <row r="42" spans="1:19" x14ac:dyDescent="0.4">
@@ -2919,16 +2919,16 @@
         <v>25</v>
       </c>
       <c r="F42" t="s">
-        <v>73</v>
-      </c>
-      <c r="G42" t="s">
-        <v>73</v>
+        <v>61</v>
+      </c>
+      <c r="G42">
+        <v>0.5</v>
       </c>
       <c r="H42" t="s">
-        <v>76</v>
-      </c>
-      <c r="I42">
-        <v>10</v>
+        <v>73</v>
+      </c>
+      <c r="I42" t="s">
+        <v>73</v>
       </c>
       <c r="J42" t="s">
         <v>73</v>
@@ -2952,7 +2952,7 @@
         <v>0</v>
       </c>
       <c r="S42" t="s">
-        <v>79</v>
+        <v>64</v>
       </c>
     </row>
     <row r="43" spans="1:19" x14ac:dyDescent="0.4">
@@ -2972,16 +2972,16 @@
         <v>25</v>
       </c>
       <c r="F43" t="s">
-        <v>73</v>
-      </c>
-      <c r="G43" t="s">
-        <v>73</v>
+        <v>65</v>
+      </c>
+      <c r="G43">
+        <v>0.1</v>
       </c>
       <c r="H43" t="s">
-        <v>80</v>
-      </c>
-      <c r="I43">
-        <v>2</v>
+        <v>73</v>
+      </c>
+      <c r="I43" t="s">
+        <v>73</v>
       </c>
       <c r="J43" t="s">
         <v>73</v>
@@ -3005,7 +3005,7 @@
         <v>0</v>
       </c>
       <c r="S43" t="s">
-        <v>81</v>
+        <v>66</v>
       </c>
     </row>
     <row r="44" spans="1:19" x14ac:dyDescent="0.4">
@@ -3025,16 +3025,16 @@
         <v>25</v>
       </c>
       <c r="F44" t="s">
-        <v>73</v>
-      </c>
-      <c r="G44" t="s">
-        <v>73</v>
+        <v>65</v>
+      </c>
+      <c r="G44">
+        <v>0.2</v>
       </c>
       <c r="H44" t="s">
-        <v>80</v>
-      </c>
-      <c r="I44">
-        <v>5</v>
+        <v>73</v>
+      </c>
+      <c r="I44" t="s">
+        <v>73</v>
       </c>
       <c r="J44" t="s">
         <v>73</v>
@@ -3058,7 +3058,7 @@
         <v>0</v>
       </c>
       <c r="S44" t="s">
-        <v>82</v>
+        <v>67</v>
       </c>
     </row>
     <row r="45" spans="1:19" x14ac:dyDescent="0.4">
@@ -3078,16 +3078,16 @@
         <v>25</v>
       </c>
       <c r="F45" t="s">
-        <v>73</v>
-      </c>
-      <c r="G45" t="s">
-        <v>73</v>
+        <v>65</v>
+      </c>
+      <c r="G45">
+        <v>0.5</v>
       </c>
       <c r="H45" t="s">
-        <v>80</v>
-      </c>
-      <c r="I45">
-        <v>10</v>
+        <v>73</v>
+      </c>
+      <c r="I45" t="s">
+        <v>73</v>
       </c>
       <c r="J45" t="s">
         <v>73</v>
@@ -3111,7 +3111,7 @@
         <v>0</v>
       </c>
       <c r="S45" t="s">
-        <v>83</v>
+        <v>68</v>
       </c>
     </row>
     <row r="46" spans="1:19" x14ac:dyDescent="0.4">
@@ -3131,16 +3131,16 @@
         <v>25</v>
       </c>
       <c r="F46" t="s">
-        <v>73</v>
-      </c>
-      <c r="G46" t="s">
-        <v>73</v>
+        <v>48</v>
+      </c>
+      <c r="G46">
+        <v>0.1</v>
       </c>
       <c r="H46" t="s">
-        <v>84</v>
-      </c>
-      <c r="I46">
-        <v>2</v>
+        <v>73</v>
+      </c>
+      <c r="I46" t="s">
+        <v>73</v>
       </c>
       <c r="J46" t="s">
         <v>73</v>
@@ -3164,7 +3164,7 @@
         <v>0</v>
       </c>
       <c r="S46" t="s">
-        <v>85</v>
+        <v>69</v>
       </c>
     </row>
     <row r="47" spans="1:19" x14ac:dyDescent="0.4">
@@ -3184,16 +3184,16 @@
         <v>25</v>
       </c>
       <c r="F47" t="s">
-        <v>73</v>
-      </c>
-      <c r="G47" t="s">
-        <v>73</v>
+        <v>48</v>
+      </c>
+      <c r="G47">
+        <v>0.2</v>
       </c>
       <c r="H47" t="s">
-        <v>84</v>
-      </c>
-      <c r="I47">
-        <v>5</v>
+        <v>73</v>
+      </c>
+      <c r="I47" t="s">
+        <v>73</v>
       </c>
       <c r="J47" t="s">
         <v>73</v>
@@ -3217,7 +3217,7 @@
         <v>0</v>
       </c>
       <c r="S47" t="s">
-        <v>86</v>
+        <v>70</v>
       </c>
     </row>
     <row r="48" spans="1:19" x14ac:dyDescent="0.4">
@@ -3237,16 +3237,16 @@
         <v>25</v>
       </c>
       <c r="F48" t="s">
-        <v>73</v>
-      </c>
-      <c r="G48" t="s">
-        <v>73</v>
+        <v>48</v>
+      </c>
+      <c r="G48">
+        <v>0.5</v>
       </c>
       <c r="H48" t="s">
-        <v>84</v>
-      </c>
-      <c r="I48">
-        <v>10</v>
+        <v>73</v>
+      </c>
+      <c r="I48" t="s">
+        <v>73</v>
       </c>
       <c r="J48" t="s">
         <v>73</v>
@@ -3270,7 +3270,7 @@
         <v>0</v>
       </c>
       <c r="S48" t="s">
-        <v>87</v>
+        <v>71</v>
       </c>
     </row>
     <row r="49" spans="1:19" x14ac:dyDescent="0.4">
@@ -3290,16 +3290,16 @@
         <v>25</v>
       </c>
       <c r="F49" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G49" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="H49" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="I49" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="J49" t="s">
         <v>73</v>
@@ -3308,13 +3308,13 @@
         <v>73</v>
       </c>
       <c r="L49" t="s">
-        <v>88</v>
+        <v>26</v>
       </c>
       <c r="M49">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="N49">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O49">
         <v>0</v>
@@ -3323,7 +3323,7 @@
         <v>0</v>
       </c>
       <c r="S49" t="s">
-        <v>89</v>
+        <v>104</v>
       </c>
     </row>
     <row r="50" spans="1:19" x14ac:dyDescent="0.4">
@@ -3364,10 +3364,10 @@
         <v>88</v>
       </c>
       <c r="M50">
-        <v>0.2</v>
-      </c>
-      <c r="N50">
-        <v>0</v>
+        <v>0.1</v>
+      </c>
+      <c r="N50" t="s">
+        <v>72</v>
       </c>
       <c r="O50">
         <v>0</v>
@@ -3376,7 +3376,7 @@
         <v>0</v>
       </c>
       <c r="S50" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="51" spans="1:19" x14ac:dyDescent="0.4">
@@ -3417,10 +3417,10 @@
         <v>88</v>
       </c>
       <c r="M51">
-        <v>0.5</v>
-      </c>
-      <c r="N51">
-        <v>0</v>
+        <v>0.2</v>
+      </c>
+      <c r="N51" t="s">
+        <v>73</v>
       </c>
       <c r="O51">
         <v>0</v>
@@ -3429,7 +3429,7 @@
         <v>0</v>
       </c>
       <c r="S51" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="52" spans="1:19" x14ac:dyDescent="0.4">
@@ -3467,13 +3467,13 @@
         <v>73</v>
       </c>
       <c r="L52" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="M52">
-        <v>0.1</v>
-      </c>
-      <c r="N52">
-        <v>0</v>
+        <v>0.5</v>
+      </c>
+      <c r="N52" t="s">
+        <v>73</v>
       </c>
       <c r="O52">
         <v>0</v>
@@ -3482,7 +3482,7 @@
         <v>0</v>
       </c>
       <c r="S52" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="53" spans="1:19" x14ac:dyDescent="0.4">
@@ -3523,10 +3523,10 @@
         <v>92</v>
       </c>
       <c r="M53">
-        <v>0.2</v>
-      </c>
-      <c r="N53">
-        <v>0</v>
+        <v>0.1</v>
+      </c>
+      <c r="N53" t="s">
+        <v>73</v>
       </c>
       <c r="O53">
         <v>0</v>
@@ -3535,7 +3535,7 @@
         <v>0</v>
       </c>
       <c r="S53" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="54" spans="1:19" x14ac:dyDescent="0.4">
@@ -3576,10 +3576,10 @@
         <v>92</v>
       </c>
       <c r="M54">
-        <v>0.5</v>
-      </c>
-      <c r="N54">
-        <v>0</v>
+        <v>0.2</v>
+      </c>
+      <c r="N54" t="s">
+        <v>73</v>
       </c>
       <c r="O54">
         <v>0</v>
@@ -3588,7 +3588,7 @@
         <v>0</v>
       </c>
       <c r="S54" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="55" spans="1:19" x14ac:dyDescent="0.4">
@@ -3626,13 +3626,13 @@
         <v>73</v>
       </c>
       <c r="L55" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="M55">
-        <v>0.1</v>
-      </c>
-      <c r="N55">
-        <v>0</v>
+        <v>0.5</v>
+      </c>
+      <c r="N55" t="s">
+        <v>73</v>
       </c>
       <c r="O55">
         <v>0</v>
@@ -3641,7 +3641,7 @@
         <v>0</v>
       </c>
       <c r="S55" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="56" spans="1:19" x14ac:dyDescent="0.4">
@@ -3682,10 +3682,10 @@
         <v>96</v>
       </c>
       <c r="M56">
-        <v>0.2</v>
-      </c>
-      <c r="N56">
-        <v>0</v>
+        <v>0.1</v>
+      </c>
+      <c r="N56" t="s">
+        <v>73</v>
       </c>
       <c r="O56">
         <v>0</v>
@@ -3694,7 +3694,7 @@
         <v>0</v>
       </c>
       <c r="S56" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="57" spans="1:19" x14ac:dyDescent="0.4">
@@ -3735,10 +3735,10 @@
         <v>96</v>
       </c>
       <c r="M57">
-        <v>0.5</v>
-      </c>
-      <c r="N57">
-        <v>0</v>
+        <v>0.2</v>
+      </c>
+      <c r="N57" t="s">
+        <v>73</v>
       </c>
       <c r="O57">
         <v>0</v>
@@ -3747,7 +3747,7 @@
         <v>0</v>
       </c>
       <c r="S57" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="58" spans="1:19" x14ac:dyDescent="0.4">
@@ -3785,13 +3785,13 @@
         <v>73</v>
       </c>
       <c r="L58" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="M58">
-        <v>0.1</v>
-      </c>
-      <c r="N58">
-        <v>0</v>
+        <v>0.5</v>
+      </c>
+      <c r="N58" t="s">
+        <v>73</v>
       </c>
       <c r="O58">
         <v>0</v>
@@ -3800,7 +3800,7 @@
         <v>0</v>
       </c>
       <c r="S58" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="59" spans="1:19" x14ac:dyDescent="0.4">
@@ -3841,10 +3841,10 @@
         <v>100</v>
       </c>
       <c r="M59">
-        <v>0.2</v>
-      </c>
-      <c r="N59">
-        <v>0</v>
+        <v>0.1</v>
+      </c>
+      <c r="N59" t="s">
+        <v>73</v>
       </c>
       <c r="O59">
         <v>0</v>
@@ -3853,7 +3853,7 @@
         <v>0</v>
       </c>
       <c r="S59" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="60" spans="1:19" x14ac:dyDescent="0.4">
@@ -3894,10 +3894,10 @@
         <v>100</v>
       </c>
       <c r="M60">
-        <v>0.5</v>
-      </c>
-      <c r="N60">
-        <v>0</v>
+        <v>0.2</v>
+      </c>
+      <c r="N60" t="s">
+        <v>73</v>
       </c>
       <c r="O60">
         <v>0</v>
@@ -3906,7 +3906,7 @@
         <v>0</v>
       </c>
       <c r="S60" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="61" spans="1:19" x14ac:dyDescent="0.4">
@@ -3944,13 +3944,13 @@
         <v>73</v>
       </c>
       <c r="L61" t="s">
-        <v>72</v>
-      </c>
-      <c r="M61" t="s">
-        <v>72</v>
-      </c>
-      <c r="N61">
-        <v>1</v>
+        <v>100</v>
+      </c>
+      <c r="M61">
+        <v>0.5</v>
+      </c>
+      <c r="N61" t="s">
+        <v>73</v>
       </c>
       <c r="O61">
         <v>0</v>
@@ -3959,7 +3959,7 @@
         <v>0</v>
       </c>
       <c r="S61" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="62" spans="1:19" x14ac:dyDescent="0.4">
@@ -3997,13 +3997,13 @@
         <v>73</v>
       </c>
       <c r="L62" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="M62" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="N62" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="O62">
         <v>1</v>

</xml_diff>

<commit_message>
Minor changes to testing sheet
</commit_message>
<xml_diff>
--- a/Test_Template.xlsx
+++ b/Test_Template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aasav\github-classroom\EMAT31530\group-project-2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A274D455-0D48-4E06-85C8-16F69B340EE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE0216D2-DA6B-4A08-96A5-90679368CCF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="25920" windowHeight="16629" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="553" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="552" uniqueCount="105">
   <si>
     <t>Test ID</t>
   </si>
@@ -67,15 +67,9 @@
     <t>Sparse Reward</t>
   </si>
   <si>
-    <t>Unnamed: 15</t>
-  </si>
-  <si>
     <t>Completed</t>
   </si>
   <si>
-    <t>Unnamed: 17</t>
-  </si>
-  <si>
     <t>Description</t>
   </si>
   <si>
@@ -338,6 +332,9 @@
   </si>
   <si>
     <t>Sparse Reward enabled</t>
+  </si>
+  <si>
+    <t>Error Message</t>
   </si>
 </sst>
 </file>
@@ -393,9 +390,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -703,7 +704,7 @@
   <dimension ref="A1:X62"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="V50" sqref="V50"/>
+      <selection activeCell="U14" sqref="U14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -755,31 +756,29 @@
         <v>14</v>
       </c>
       <c r="P1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q1" s="2"/>
+      <c r="R1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="T1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="V1" s="1" t="s">
+      <c r="W1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="X1" s="1" t="s">
         <v>21</v>
-      </c>
-      <c r="W1" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="X1" s="1" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:24" x14ac:dyDescent="0.4">
@@ -787,7 +786,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C2">
         <v>5</v>
@@ -796,43 +795,43 @@
         <v>5</v>
       </c>
       <c r="E2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2" t="s">
         <v>25</v>
-      </c>
-      <c r="F2" t="s">
-        <v>26</v>
-      </c>
-      <c r="G2">
-        <v>0</v>
-      </c>
-      <c r="H2" t="s">
-        <v>27</v>
       </c>
       <c r="I2">
         <v>2</v>
       </c>
       <c r="J2" t="s">
+        <v>24</v>
+      </c>
+      <c r="K2">
+        <v>0</v>
+      </c>
+      <c r="L2" t="s">
+        <v>24</v>
+      </c>
+      <c r="M2">
+        <v>0</v>
+      </c>
+      <c r="N2">
+        <v>0</v>
+      </c>
+      <c r="O2">
+        <v>0</v>
+      </c>
+      <c r="P2" t="s">
         <v>26</v>
       </c>
-      <c r="K2">
-        <v>0</v>
-      </c>
-      <c r="L2" t="s">
-        <v>26</v>
-      </c>
-      <c r="M2">
-        <v>0</v>
-      </c>
-      <c r="N2">
-        <v>0</v>
-      </c>
-      <c r="O2">
-        <v>0</v>
-      </c>
-      <c r="Q2">
-        <v>0</v>
-      </c>
-      <c r="S2" t="s">
-        <v>28</v>
+      <c r="R2">
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:24" x14ac:dyDescent="0.4">
@@ -840,7 +839,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C3">
         <v>5</v>
@@ -849,28 +848,28 @@
         <v>10</v>
       </c>
       <c r="E3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F3" t="s">
+        <v>24</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3" t="s">
         <v>25</v>
-      </c>
-      <c r="F3" t="s">
-        <v>26</v>
-      </c>
-      <c r="G3">
-        <v>0</v>
-      </c>
-      <c r="H3" t="s">
-        <v>27</v>
       </c>
       <c r="I3">
         <v>2</v>
       </c>
       <c r="J3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="K3">
         <v>0</v>
       </c>
       <c r="L3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="M3">
         <v>0</v>
@@ -881,11 +880,11 @@
       <c r="O3">
         <v>0</v>
       </c>
-      <c r="Q3">
-        <v>0</v>
-      </c>
-      <c r="S3" t="s">
-        <v>29</v>
+      <c r="P3" t="s">
+        <v>27</v>
+      </c>
+      <c r="R3">
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:24" x14ac:dyDescent="0.4">
@@ -893,7 +892,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C4">
         <v>10</v>
@@ -902,28 +901,28 @@
         <v>5</v>
       </c>
       <c r="E4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F4" t="s">
+        <v>24</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4" t="s">
         <v>25</v>
-      </c>
-      <c r="F4" t="s">
-        <v>26</v>
-      </c>
-      <c r="G4">
-        <v>0</v>
-      </c>
-      <c r="H4" t="s">
-        <v>27</v>
       </c>
       <c r="I4">
         <v>2</v>
       </c>
       <c r="J4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="K4">
         <v>0</v>
       </c>
       <c r="L4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="M4">
         <v>0</v>
@@ -934,11 +933,11 @@
       <c r="O4">
         <v>0</v>
       </c>
-      <c r="Q4">
-        <v>0</v>
-      </c>
-      <c r="S4" t="s">
-        <v>30</v>
+      <c r="P4" t="s">
+        <v>28</v>
+      </c>
+      <c r="R4">
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:24" x14ac:dyDescent="0.4">
@@ -946,7 +945,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C5">
         <v>10</v>
@@ -955,28 +954,28 @@
         <v>10</v>
       </c>
       <c r="E5" t="s">
+        <v>23</v>
+      </c>
+      <c r="F5" t="s">
+        <v>24</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5" t="s">
         <v>25</v>
-      </c>
-      <c r="F5" t="s">
-        <v>26</v>
-      </c>
-      <c r="G5">
-        <v>0</v>
-      </c>
-      <c r="H5" t="s">
-        <v>27</v>
       </c>
       <c r="I5">
         <v>2</v>
       </c>
       <c r="J5" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="K5">
         <v>0</v>
       </c>
       <c r="L5" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="M5">
         <v>0</v>
@@ -987,11 +986,11 @@
       <c r="O5">
         <v>0</v>
       </c>
-      <c r="Q5">
-        <v>0</v>
-      </c>
-      <c r="S5" t="s">
-        <v>31</v>
+      <c r="P5" t="s">
+        <v>29</v>
+      </c>
+      <c r="R5">
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:24" x14ac:dyDescent="0.4">
@@ -999,7 +998,7 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C6">
         <v>20</v>
@@ -1008,28 +1007,28 @@
         <v>20</v>
       </c>
       <c r="E6" t="s">
+        <v>23</v>
+      </c>
+      <c r="F6" t="s">
+        <v>24</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6" t="s">
         <v>25</v>
-      </c>
-      <c r="F6" t="s">
-        <v>26</v>
-      </c>
-      <c r="G6">
-        <v>0</v>
-      </c>
-      <c r="H6" t="s">
-        <v>27</v>
       </c>
       <c r="I6">
         <v>2</v>
       </c>
       <c r="J6" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="K6">
         <v>0</v>
       </c>
       <c r="L6" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="M6">
         <v>0</v>
@@ -1040,11 +1039,11 @@
       <c r="O6">
         <v>0</v>
       </c>
-      <c r="Q6">
-        <v>0</v>
-      </c>
-      <c r="S6" t="s">
-        <v>32</v>
+      <c r="P6" t="s">
+        <v>30</v>
+      </c>
+      <c r="R6">
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:24" x14ac:dyDescent="0.4">
@@ -1052,7 +1051,7 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C7">
         <v>20</v>
@@ -1061,28 +1060,28 @@
         <v>20</v>
       </c>
       <c r="E7" t="s">
+        <v>23</v>
+      </c>
+      <c r="F7" t="s">
+        <v>24</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7" t="s">
         <v>25</v>
-      </c>
-      <c r="F7" t="s">
-        <v>26</v>
-      </c>
-      <c r="G7">
-        <v>0</v>
-      </c>
-      <c r="H7" t="s">
-        <v>27</v>
       </c>
       <c r="I7">
         <v>5</v>
       </c>
       <c r="J7" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="K7">
         <v>0</v>
       </c>
       <c r="L7" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="M7">
         <v>0</v>
@@ -1093,11 +1092,11 @@
       <c r="O7">
         <v>0</v>
       </c>
-      <c r="Q7">
-        <v>0</v>
-      </c>
-      <c r="S7" t="s">
-        <v>74</v>
+      <c r="P7" t="s">
+        <v>72</v>
+      </c>
+      <c r="R7">
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:24" x14ac:dyDescent="0.4">
@@ -1105,7 +1104,7 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C8">
         <v>20</v>
@@ -1114,28 +1113,28 @@
         <v>20</v>
       </c>
       <c r="E8" t="s">
+        <v>23</v>
+      </c>
+      <c r="F8" t="s">
+        <v>24</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+      <c r="H8" t="s">
         <v>25</v>
-      </c>
-      <c r="F8" t="s">
-        <v>26</v>
-      </c>
-      <c r="G8">
-        <v>0</v>
-      </c>
-      <c r="H8" t="s">
-        <v>27</v>
       </c>
       <c r="I8">
         <v>10</v>
       </c>
       <c r="J8" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="K8">
         <v>0</v>
       </c>
       <c r="L8" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="M8">
         <v>0</v>
@@ -1146,11 +1145,11 @@
       <c r="O8">
         <v>0</v>
       </c>
-      <c r="Q8">
-        <v>0</v>
-      </c>
-      <c r="S8" t="s">
-        <v>75</v>
+      <c r="P8" t="s">
+        <v>73</v>
+      </c>
+      <c r="R8">
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:24" x14ac:dyDescent="0.4">
@@ -1158,7 +1157,7 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C9">
         <v>20</v>
@@ -1167,28 +1166,28 @@
         <v>20</v>
       </c>
       <c r="E9" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F9" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="G9">
         <v>0</v>
       </c>
       <c r="H9" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="I9">
         <v>2</v>
       </c>
       <c r="J9" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="K9">
         <v>0</v>
       </c>
       <c r="L9" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="M9">
         <v>0</v>
@@ -1199,11 +1198,11 @@
       <c r="O9">
         <v>0</v>
       </c>
-      <c r="Q9">
-        <v>0</v>
-      </c>
-      <c r="S9" t="s">
-        <v>77</v>
+      <c r="P9" t="s">
+        <v>75</v>
+      </c>
+      <c r="R9">
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:24" x14ac:dyDescent="0.4">
@@ -1211,7 +1210,7 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C10">
         <v>20</v>
@@ -1220,28 +1219,28 @@
         <v>20</v>
       </c>
       <c r="E10" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F10" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="G10">
         <v>0</v>
       </c>
       <c r="H10" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="I10">
         <v>5</v>
       </c>
       <c r="J10" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="K10">
         <v>0</v>
       </c>
       <c r="L10" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="M10">
         <v>0</v>
@@ -1252,11 +1251,11 @@
       <c r="O10">
         <v>0</v>
       </c>
-      <c r="Q10">
-        <v>0</v>
-      </c>
-      <c r="S10" t="s">
-        <v>78</v>
+      <c r="P10" t="s">
+        <v>76</v>
+      </c>
+      <c r="R10">
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:24" x14ac:dyDescent="0.4">
@@ -1264,7 +1263,7 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C11">
         <v>20</v>
@@ -1273,28 +1272,28 @@
         <v>20</v>
       </c>
       <c r="E11" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F11" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="G11">
         <v>0</v>
       </c>
       <c r="H11" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="I11">
         <v>10</v>
       </c>
       <c r="J11" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="K11">
         <v>0</v>
       </c>
       <c r="L11" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="M11">
         <v>0</v>
@@ -1305,11 +1304,11 @@
       <c r="O11">
         <v>0</v>
       </c>
-      <c r="Q11">
-        <v>0</v>
-      </c>
-      <c r="S11" t="s">
-        <v>79</v>
+      <c r="P11" t="s">
+        <v>77</v>
+      </c>
+      <c r="R11">
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:24" x14ac:dyDescent="0.4">
@@ -1317,7 +1316,7 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C12">
         <v>20</v>
@@ -1326,28 +1325,28 @@
         <v>20</v>
       </c>
       <c r="E12" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F12" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="G12">
         <v>0</v>
       </c>
       <c r="H12" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="I12">
         <v>2</v>
       </c>
       <c r="J12" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="K12">
         <v>0</v>
       </c>
       <c r="L12" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="M12">
         <v>0</v>
@@ -1358,11 +1357,11 @@
       <c r="O12">
         <v>0</v>
       </c>
-      <c r="Q12">
-        <v>0</v>
-      </c>
-      <c r="S12" t="s">
-        <v>81</v>
+      <c r="P12" t="s">
+        <v>79</v>
+      </c>
+      <c r="R12">
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:24" x14ac:dyDescent="0.4">
@@ -1370,7 +1369,7 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C13">
         <v>20</v>
@@ -1379,28 +1378,28 @@
         <v>20</v>
       </c>
       <c r="E13" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F13" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="G13">
         <v>0</v>
       </c>
       <c r="H13" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="I13">
         <v>5</v>
       </c>
       <c r="J13" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="K13">
         <v>0</v>
       </c>
       <c r="L13" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="M13">
         <v>0</v>
@@ -1411,11 +1410,11 @@
       <c r="O13">
         <v>0</v>
       </c>
-      <c r="Q13">
-        <v>0</v>
-      </c>
-      <c r="S13" t="s">
-        <v>82</v>
+      <c r="P13" t="s">
+        <v>80</v>
+      </c>
+      <c r="R13">
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:24" x14ac:dyDescent="0.4">
@@ -1423,7 +1422,7 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C14">
         <v>20</v>
@@ -1432,28 +1431,28 @@
         <v>20</v>
       </c>
       <c r="E14" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F14" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="G14">
         <v>0</v>
       </c>
       <c r="H14" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="I14">
         <v>10</v>
       </c>
       <c r="J14" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="K14">
         <v>0</v>
       </c>
       <c r="L14" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="M14">
         <v>0</v>
@@ -1464,11 +1463,11 @@
       <c r="O14">
         <v>0</v>
       </c>
-      <c r="Q14">
-        <v>0</v>
-      </c>
-      <c r="S14" t="s">
-        <v>83</v>
+      <c r="P14" t="s">
+        <v>81</v>
+      </c>
+      <c r="R14">
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:24" x14ac:dyDescent="0.4">
@@ -1476,7 +1475,7 @@
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C15">
         <v>20</v>
@@ -1485,28 +1484,28 @@
         <v>20</v>
       </c>
       <c r="E15" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F15" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="G15">
         <v>0</v>
       </c>
       <c r="H15" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="I15">
         <v>2</v>
       </c>
       <c r="J15" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="K15">
         <v>0</v>
       </c>
       <c r="L15" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="M15">
         <v>0</v>
@@ -1517,11 +1516,11 @@
       <c r="O15">
         <v>0</v>
       </c>
-      <c r="Q15">
-        <v>0</v>
-      </c>
-      <c r="S15" t="s">
-        <v>85</v>
+      <c r="P15" t="s">
+        <v>83</v>
+      </c>
+      <c r="R15">
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:24" x14ac:dyDescent="0.4">
@@ -1529,7 +1528,7 @@
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C16">
         <v>20</v>
@@ -1538,28 +1537,28 @@
         <v>20</v>
       </c>
       <c r="E16" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F16" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="G16">
         <v>0</v>
       </c>
       <c r="H16" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="I16">
         <v>5</v>
       </c>
       <c r="J16" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="K16">
         <v>0</v>
       </c>
       <c r="L16" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="M16">
         <v>0</v>
@@ -1570,19 +1569,19 @@
       <c r="O16">
         <v>0</v>
       </c>
-      <c r="Q16">
-        <v>0</v>
-      </c>
-      <c r="S16" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.4">
+      <c r="P16" t="s">
+        <v>84</v>
+      </c>
+      <c r="R16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A17">
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C17">
         <v>20</v>
@@ -1591,28 +1590,28 @@
         <v>20</v>
       </c>
       <c r="E17" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F17" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="G17">
         <v>0</v>
       </c>
       <c r="H17" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="I17">
         <v>10</v>
       </c>
       <c r="J17" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="K17">
         <v>0</v>
       </c>
       <c r="L17" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="M17">
         <v>0</v>
@@ -1623,19 +1622,19 @@
       <c r="O17">
         <v>0</v>
       </c>
-      <c r="Q17">
-        <v>0</v>
-      </c>
-      <c r="S17" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.4">
+      <c r="P17" t="s">
+        <v>85</v>
+      </c>
+      <c r="R17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A18">
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C18">
         <v>20</v>
@@ -1644,28 +1643,28 @@
         <v>20</v>
       </c>
       <c r="E18" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F18" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="G18">
         <v>0</v>
       </c>
       <c r="H18" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="I18" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="J18" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="K18">
         <v>0.2</v>
       </c>
       <c r="L18" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="M18">
         <v>0</v>
@@ -1676,19 +1675,19 @@
       <c r="O18">
         <v>0</v>
       </c>
-      <c r="Q18">
-        <v>0</v>
-      </c>
-      <c r="S18" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.4">
+      <c r="P18" t="s">
+        <v>32</v>
+      </c>
+      <c r="R18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A19">
         <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C19">
         <v>20</v>
@@ -1697,28 +1696,28 @@
         <v>20</v>
       </c>
       <c r="E19" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F19" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="G19">
         <v>0</v>
       </c>
       <c r="H19" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="I19" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="J19" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="K19">
         <v>0.5</v>
       </c>
       <c r="L19" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="M19">
         <v>0</v>
@@ -1729,19 +1728,19 @@
       <c r="O19">
         <v>0</v>
       </c>
-      <c r="Q19">
-        <v>0</v>
-      </c>
-      <c r="S19" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.4">
+      <c r="P19" t="s">
+        <v>33</v>
+      </c>
+      <c r="R19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A20">
         <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C20">
         <v>20</v>
@@ -1750,28 +1749,28 @@
         <v>20</v>
       </c>
       <c r="E20" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F20" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="G20">
         <v>0</v>
       </c>
       <c r="H20" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="I20" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="J20" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="K20">
         <v>0.7</v>
       </c>
       <c r="L20" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="M20">
         <v>0</v>
@@ -1782,19 +1781,19 @@
       <c r="O20">
         <v>0</v>
       </c>
-      <c r="Q20">
-        <v>0</v>
-      </c>
-      <c r="S20" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.4">
+      <c r="P20" t="s">
+        <v>34</v>
+      </c>
+      <c r="R20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A21">
         <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C21">
         <v>20</v>
@@ -1803,28 +1802,28 @@
         <v>20</v>
       </c>
       <c r="E21" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F21" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="G21">
         <v>0</v>
       </c>
       <c r="H21" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="I21" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="J21" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="K21">
         <v>0.9</v>
       </c>
       <c r="L21" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="M21">
         <v>0</v>
@@ -1835,19 +1834,19 @@
       <c r="O21">
         <v>0</v>
       </c>
-      <c r="Q21">
-        <v>0</v>
-      </c>
-      <c r="S21" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.4">
+      <c r="P21" t="s">
+        <v>35</v>
+      </c>
+      <c r="R21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A22">
         <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C22">
         <v>20</v>
@@ -1856,28 +1855,28 @@
         <v>20</v>
       </c>
       <c r="E22" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F22" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="G22">
         <v>0</v>
       </c>
       <c r="H22" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="I22" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="J22" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="K22">
         <v>0.2</v>
       </c>
       <c r="L22" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="M22">
         <v>0</v>
@@ -1888,19 +1887,19 @@
       <c r="O22">
         <v>0</v>
       </c>
-      <c r="Q22">
-        <v>0</v>
-      </c>
-      <c r="S22" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.4">
+      <c r="P22" t="s">
+        <v>37</v>
+      </c>
+      <c r="R22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A23">
         <v>21</v>
       </c>
       <c r="B23" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C23">
         <v>20</v>
@@ -1909,28 +1908,28 @@
         <v>20</v>
       </c>
       <c r="E23" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F23" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="G23">
         <v>0</v>
       </c>
       <c r="H23" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="I23" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="J23" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="K23">
         <v>0.5</v>
       </c>
       <c r="L23" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="M23">
         <v>0</v>
@@ -1941,19 +1940,19 @@
       <c r="O23">
         <v>0</v>
       </c>
-      <c r="Q23">
-        <v>0</v>
-      </c>
-      <c r="S23" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.4">
+      <c r="P23" t="s">
+        <v>38</v>
+      </c>
+      <c r="R23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A24">
         <v>22</v>
       </c>
       <c r="B24" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C24">
         <v>20</v>
@@ -1962,28 +1961,28 @@
         <v>20</v>
       </c>
       <c r="E24" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F24" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="G24">
         <v>0</v>
       </c>
       <c r="H24" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="I24" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="J24" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="K24">
         <v>0.7</v>
       </c>
       <c r="L24" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="M24">
         <v>0</v>
@@ -1994,19 +1993,19 @@
       <c r="O24">
         <v>0</v>
       </c>
-      <c r="Q24">
-        <v>0</v>
-      </c>
-      <c r="S24" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="25" spans="1:19" x14ac:dyDescent="0.4">
+      <c r="P24" t="s">
+        <v>39</v>
+      </c>
+      <c r="R24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A25">
         <v>23</v>
       </c>
       <c r="B25" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C25">
         <v>20</v>
@@ -2015,28 +2014,28 @@
         <v>20</v>
       </c>
       <c r="E25" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F25" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="G25">
         <v>0</v>
       </c>
       <c r="H25" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="I25" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="J25" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="K25">
         <v>0.9</v>
       </c>
       <c r="L25" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="M25">
         <v>0</v>
@@ -2047,19 +2046,19 @@
       <c r="O25">
         <v>0</v>
       </c>
-      <c r="Q25">
-        <v>0</v>
-      </c>
-      <c r="S25" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="26" spans="1:19" x14ac:dyDescent="0.4">
+      <c r="P25" t="s">
+        <v>40</v>
+      </c>
+      <c r="R25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A26">
         <v>24</v>
       </c>
       <c r="B26" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C26">
         <v>20</v>
@@ -2068,28 +2067,28 @@
         <v>20</v>
       </c>
       <c r="E26" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F26" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="G26">
         <v>0</v>
       </c>
       <c r="H26" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="I26" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="J26" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="K26">
         <v>0.2</v>
       </c>
       <c r="L26" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="M26">
         <v>0</v>
@@ -2100,19 +2099,19 @@
       <c r="O26">
         <v>0</v>
       </c>
-      <c r="Q26">
-        <v>0</v>
-      </c>
-      <c r="S26" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="27" spans="1:19" x14ac:dyDescent="0.4">
+      <c r="P26" t="s">
+        <v>42</v>
+      </c>
+      <c r="R26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A27">
         <v>25</v>
       </c>
       <c r="B27" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C27">
         <v>20</v>
@@ -2121,28 +2120,28 @@
         <v>20</v>
       </c>
       <c r="E27" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F27" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="G27">
         <v>0</v>
       </c>
       <c r="H27" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="I27" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="J27" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="K27">
         <v>0.5</v>
       </c>
       <c r="L27" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="M27">
         <v>0</v>
@@ -2153,19 +2152,19 @@
       <c r="O27">
         <v>0</v>
       </c>
-      <c r="Q27">
-        <v>0</v>
-      </c>
-      <c r="S27" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="28" spans="1:19" x14ac:dyDescent="0.4">
+      <c r="P27" t="s">
+        <v>43</v>
+      </c>
+      <c r="R27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A28">
         <v>26</v>
       </c>
       <c r="B28" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C28">
         <v>20</v>
@@ -2174,28 +2173,28 @@
         <v>20</v>
       </c>
       <c r="E28" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F28" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="G28">
         <v>0</v>
       </c>
       <c r="H28" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="I28" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="J28" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="K28">
         <v>0.7</v>
       </c>
       <c r="L28" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="M28">
         <v>0</v>
@@ -2206,19 +2205,19 @@
       <c r="O28">
         <v>0</v>
       </c>
-      <c r="Q28">
-        <v>0</v>
-      </c>
-      <c r="S28" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="29" spans="1:19" x14ac:dyDescent="0.4">
+      <c r="P28" t="s">
+        <v>44</v>
+      </c>
+      <c r="R28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A29">
         <v>27</v>
       </c>
       <c r="B29" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C29">
         <v>20</v>
@@ -2227,28 +2226,28 @@
         <v>20</v>
       </c>
       <c r="E29" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F29" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="G29">
         <v>0</v>
       </c>
       <c r="H29" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="I29" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="J29" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="K29">
         <v>0.9</v>
       </c>
       <c r="L29" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="M29">
         <v>0</v>
@@ -2259,19 +2258,19 @@
       <c r="O29">
         <v>0</v>
       </c>
-      <c r="Q29">
-        <v>0</v>
-      </c>
-      <c r="S29" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="30" spans="1:19" x14ac:dyDescent="0.4">
+      <c r="P29" t="s">
+        <v>45</v>
+      </c>
+      <c r="R29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A30">
         <v>28</v>
       </c>
       <c r="B30" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C30">
         <v>20</v>
@@ -2280,28 +2279,28 @@
         <v>20</v>
       </c>
       <c r="E30" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F30" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="G30">
         <v>0</v>
       </c>
       <c r="H30" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="I30" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="J30" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="K30">
         <v>0.2</v>
       </c>
       <c r="L30" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="M30">
         <v>0</v>
@@ -2312,19 +2311,19 @@
       <c r="O30">
         <v>0</v>
       </c>
-      <c r="Q30">
-        <v>0</v>
-      </c>
-      <c r="S30" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="31" spans="1:19" x14ac:dyDescent="0.4">
+      <c r="P30" t="s">
+        <v>47</v>
+      </c>
+      <c r="R30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A31">
         <v>29</v>
       </c>
       <c r="B31" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C31">
         <v>20</v>
@@ -2333,28 +2332,28 @@
         <v>20</v>
       </c>
       <c r="E31" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F31" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="G31">
         <v>0</v>
       </c>
       <c r="H31" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="I31" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="J31" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="K31">
         <v>0.5</v>
       </c>
       <c r="L31" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="M31">
         <v>0</v>
@@ -2365,19 +2364,19 @@
       <c r="O31">
         <v>0</v>
       </c>
-      <c r="Q31">
-        <v>0</v>
-      </c>
-      <c r="S31" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="32" spans="1:19" x14ac:dyDescent="0.4">
+      <c r="P31" t="s">
+        <v>48</v>
+      </c>
+      <c r="R31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A32">
         <v>30</v>
       </c>
       <c r="B32" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C32">
         <v>20</v>
@@ -2386,28 +2385,28 @@
         <v>20</v>
       </c>
       <c r="E32" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F32" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="G32">
         <v>0</v>
       </c>
       <c r="H32" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="I32" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="J32" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="K32">
         <v>0.7</v>
       </c>
       <c r="L32" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="M32">
         <v>0</v>
@@ -2418,19 +2417,19 @@
       <c r="O32">
         <v>0</v>
       </c>
-      <c r="Q32">
-        <v>0</v>
-      </c>
-      <c r="S32" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="33" spans="1:19" x14ac:dyDescent="0.4">
+      <c r="P32" t="s">
+        <v>49</v>
+      </c>
+      <c r="R32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A33">
         <v>31</v>
       </c>
       <c r="B33" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C33">
         <v>20</v>
@@ -2439,28 +2438,28 @@
         <v>20</v>
       </c>
       <c r="E33" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F33" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="G33">
         <v>0</v>
       </c>
       <c r="H33" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="I33" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="J33" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="K33">
         <v>0.9</v>
       </c>
       <c r="L33" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="M33">
         <v>0</v>
@@ -2471,19 +2470,19 @@
       <c r="O33">
         <v>0</v>
       </c>
-      <c r="Q33">
-        <v>0</v>
-      </c>
-      <c r="S33" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="34" spans="1:19" x14ac:dyDescent="0.4">
+      <c r="P33" t="s">
+        <v>50</v>
+      </c>
+      <c r="R33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A34">
         <v>32</v>
       </c>
       <c r="B34" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C34">
         <v>20</v>
@@ -2492,28 +2491,28 @@
         <v>20</v>
       </c>
       <c r="E34" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F34" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="G34">
         <v>0.1</v>
       </c>
       <c r="H34" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="I34" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="J34" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="K34" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="L34" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="M34">
         <v>0</v>
@@ -2524,19 +2523,19 @@
       <c r="O34">
         <v>0</v>
       </c>
-      <c r="Q34">
-        <v>0</v>
-      </c>
-      <c r="S34" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="35" spans="1:19" x14ac:dyDescent="0.4">
+      <c r="P34" t="s">
+        <v>52</v>
+      </c>
+      <c r="R34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A35">
         <v>33</v>
       </c>
       <c r="B35" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C35">
         <v>20</v>
@@ -2545,28 +2544,28 @@
         <v>20</v>
       </c>
       <c r="E35" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F35" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="G35">
         <v>0.2</v>
       </c>
       <c r="H35" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="I35" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="J35" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="K35" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="L35" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="M35">
         <v>0</v>
@@ -2577,19 +2576,19 @@
       <c r="O35">
         <v>0</v>
       </c>
-      <c r="Q35">
-        <v>0</v>
-      </c>
-      <c r="S35" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="36" spans="1:19" x14ac:dyDescent="0.4">
+      <c r="P35" t="s">
+        <v>53</v>
+      </c>
+      <c r="R35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A36">
         <v>34</v>
       </c>
       <c r="B36" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C36">
         <v>20</v>
@@ -2598,28 +2597,28 @@
         <v>20</v>
       </c>
       <c r="E36" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F36" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="G36">
         <v>0.5</v>
       </c>
       <c r="H36" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="I36" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="J36" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="K36" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="L36" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="M36">
         <v>0</v>
@@ -2630,19 +2629,19 @@
       <c r="O36">
         <v>0</v>
       </c>
-      <c r="Q36">
-        <v>0</v>
-      </c>
-      <c r="S36" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="37" spans="1:19" x14ac:dyDescent="0.4">
+      <c r="P36" t="s">
+        <v>54</v>
+      </c>
+      <c r="R36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A37">
         <v>35</v>
       </c>
       <c r="B37" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C37">
         <v>20</v>
@@ -2651,28 +2650,28 @@
         <v>20</v>
       </c>
       <c r="E37" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F37" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="G37">
         <v>0.1</v>
       </c>
       <c r="H37" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="I37" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="J37" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="K37" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="L37" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="M37">
         <v>0</v>
@@ -2683,19 +2682,19 @@
       <c r="O37">
         <v>0</v>
       </c>
-      <c r="Q37">
-        <v>0</v>
-      </c>
-      <c r="S37" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="38" spans="1:19" x14ac:dyDescent="0.4">
+      <c r="P37" t="s">
+        <v>56</v>
+      </c>
+      <c r="R37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A38">
         <v>36</v>
       </c>
       <c r="B38" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C38">
         <v>20</v>
@@ -2704,28 +2703,28 @@
         <v>20</v>
       </c>
       <c r="E38" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F38" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="G38">
         <v>0.2</v>
       </c>
       <c r="H38" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="I38" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="J38" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="K38" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="L38" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="M38">
         <v>0</v>
@@ -2736,19 +2735,19 @@
       <c r="O38">
         <v>0</v>
       </c>
-      <c r="Q38">
-        <v>0</v>
-      </c>
-      <c r="S38" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="39" spans="1:19" x14ac:dyDescent="0.4">
+      <c r="P38" t="s">
+        <v>57</v>
+      </c>
+      <c r="R38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A39">
         <v>37</v>
       </c>
       <c r="B39" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C39">
         <v>20</v>
@@ -2757,28 +2756,28 @@
         <v>20</v>
       </c>
       <c r="E39" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F39" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="G39">
         <v>0.5</v>
       </c>
       <c r="H39" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="I39" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="J39" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="K39" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="L39" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="M39">
         <v>0</v>
@@ -2789,19 +2788,19 @@
       <c r="O39">
         <v>0</v>
       </c>
-      <c r="Q39">
-        <v>0</v>
-      </c>
-      <c r="S39" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="40" spans="1:19" x14ac:dyDescent="0.4">
+      <c r="P39" t="s">
+        <v>58</v>
+      </c>
+      <c r="R39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A40">
         <v>38</v>
       </c>
       <c r="B40" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C40">
         <v>20</v>
@@ -2810,28 +2809,28 @@
         <v>20</v>
       </c>
       <c r="E40" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F40" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="G40">
         <v>0.1</v>
       </c>
       <c r="H40" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="I40" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="J40" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="K40" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="L40" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="M40">
         <v>0</v>
@@ -2842,19 +2841,19 @@
       <c r="O40">
         <v>0</v>
       </c>
-      <c r="Q40">
-        <v>0</v>
-      </c>
-      <c r="S40" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="41" spans="1:19" x14ac:dyDescent="0.4">
+      <c r="P40" t="s">
+        <v>60</v>
+      </c>
+      <c r="R40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A41">
         <v>39</v>
       </c>
       <c r="B41" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C41">
         <v>20</v>
@@ -2863,28 +2862,28 @@
         <v>20</v>
       </c>
       <c r="E41" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F41" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="G41">
         <v>0.2</v>
       </c>
       <c r="H41" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="I41" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="J41" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="K41" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="L41" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="M41">
         <v>0</v>
@@ -2895,19 +2894,19 @@
       <c r="O41">
         <v>0</v>
       </c>
-      <c r="Q41">
-        <v>0</v>
-      </c>
-      <c r="S41" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="42" spans="1:19" x14ac:dyDescent="0.4">
+      <c r="P41" t="s">
+        <v>61</v>
+      </c>
+      <c r="R41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A42">
         <v>40</v>
       </c>
       <c r="B42" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C42">
         <v>20</v>
@@ -2916,28 +2915,28 @@
         <v>20</v>
       </c>
       <c r="E42" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F42" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="G42">
         <v>0.5</v>
       </c>
       <c r="H42" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="I42" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="J42" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="K42" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="L42" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="M42">
         <v>0</v>
@@ -2948,19 +2947,19 @@
       <c r="O42">
         <v>0</v>
       </c>
-      <c r="Q42">
-        <v>0</v>
-      </c>
-      <c r="S42" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="43" spans="1:19" x14ac:dyDescent="0.4">
+      <c r="P42" t="s">
+        <v>62</v>
+      </c>
+      <c r="R42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A43">
         <v>41</v>
       </c>
       <c r="B43" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C43">
         <v>20</v>
@@ -2969,28 +2968,28 @@
         <v>20</v>
       </c>
       <c r="E43" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F43" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="G43">
         <v>0.1</v>
       </c>
       <c r="H43" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="I43" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="J43" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="K43" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="L43" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="M43">
         <v>0</v>
@@ -3001,19 +3000,19 @@
       <c r="O43">
         <v>0</v>
       </c>
-      <c r="Q43">
-        <v>0</v>
-      </c>
-      <c r="S43" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="44" spans="1:19" x14ac:dyDescent="0.4">
+      <c r="P43" t="s">
+        <v>64</v>
+      </c>
+      <c r="R43">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A44">
         <v>42</v>
       </c>
       <c r="B44" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C44">
         <v>20</v>
@@ -3022,28 +3021,28 @@
         <v>20</v>
       </c>
       <c r="E44" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F44" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="G44">
         <v>0.2</v>
       </c>
       <c r="H44" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="I44" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="J44" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="K44" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="L44" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="M44">
         <v>0</v>
@@ -3054,19 +3053,19 @@
       <c r="O44">
         <v>0</v>
       </c>
-      <c r="Q44">
-        <v>0</v>
-      </c>
-      <c r="S44" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="45" spans="1:19" x14ac:dyDescent="0.4">
+      <c r="P44" t="s">
+        <v>65</v>
+      </c>
+      <c r="R44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A45">
         <v>43</v>
       </c>
       <c r="B45" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C45">
         <v>20</v>
@@ -3075,28 +3074,28 @@
         <v>20</v>
       </c>
       <c r="E45" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F45" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="G45">
         <v>0.5</v>
       </c>
       <c r="H45" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="I45" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="J45" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="K45" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="L45" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="M45">
         <v>0</v>
@@ -3107,19 +3106,19 @@
       <c r="O45">
         <v>0</v>
       </c>
-      <c r="Q45">
-        <v>0</v>
-      </c>
-      <c r="S45" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="46" spans="1:19" x14ac:dyDescent="0.4">
+      <c r="P45" t="s">
+        <v>66</v>
+      </c>
+      <c r="R45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A46">
         <v>44</v>
       </c>
       <c r="B46" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C46">
         <v>20</v>
@@ -3128,28 +3127,28 @@
         <v>20</v>
       </c>
       <c r="E46" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F46" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="G46">
         <v>0.1</v>
       </c>
       <c r="H46" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="I46" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="J46" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="K46" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="L46" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="M46">
         <v>0</v>
@@ -3160,19 +3159,19 @@
       <c r="O46">
         <v>0</v>
       </c>
-      <c r="Q46">
-        <v>0</v>
-      </c>
-      <c r="S46" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="47" spans="1:19" x14ac:dyDescent="0.4">
+      <c r="P46" t="s">
+        <v>67</v>
+      </c>
+      <c r="R46">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A47">
         <v>45</v>
       </c>
       <c r="B47" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C47">
         <v>20</v>
@@ -3181,28 +3180,28 @@
         <v>20</v>
       </c>
       <c r="E47" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F47" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="G47">
         <v>0.2</v>
       </c>
       <c r="H47" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="I47" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="J47" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="K47" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="L47" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="M47">
         <v>0</v>
@@ -3213,19 +3212,19 @@
       <c r="O47">
         <v>0</v>
       </c>
-      <c r="Q47">
-        <v>0</v>
-      </c>
-      <c r="S47" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="48" spans="1:19" x14ac:dyDescent="0.4">
+      <c r="P47" t="s">
+        <v>68</v>
+      </c>
+      <c r="R47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A48">
         <v>46</v>
       </c>
       <c r="B48" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C48">
         <v>20</v>
@@ -3234,28 +3233,28 @@
         <v>20</v>
       </c>
       <c r="E48" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F48" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="G48">
         <v>0.5</v>
       </c>
       <c r="H48" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="I48" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="J48" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="K48" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="L48" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="M48">
         <v>0</v>
@@ -3266,19 +3265,19 @@
       <c r="O48">
         <v>0</v>
       </c>
-      <c r="Q48">
-        <v>0</v>
-      </c>
-      <c r="S48" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="49" spans="1:19" x14ac:dyDescent="0.4">
+      <c r="P48" t="s">
+        <v>69</v>
+      </c>
+      <c r="R48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A49">
         <v>47</v>
       </c>
       <c r="B49" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C49">
         <v>20</v>
@@ -3287,28 +3286,28 @@
         <v>20</v>
       </c>
       <c r="E49" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F49" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="G49" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="H49" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="I49" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="J49" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="K49" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="L49" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="M49">
         <v>0</v>
@@ -3319,19 +3318,19 @@
       <c r="O49">
         <v>0</v>
       </c>
-      <c r="Q49">
-        <v>0</v>
-      </c>
-      <c r="S49" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="50" spans="1:19" x14ac:dyDescent="0.4">
+      <c r="P49" t="s">
+        <v>102</v>
+      </c>
+      <c r="R49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A50">
         <v>48</v>
       </c>
       <c r="B50" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C50">
         <v>20</v>
@@ -3340,51 +3339,51 @@
         <v>20</v>
       </c>
       <c r="E50" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F50" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="G50" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="H50" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="I50" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="J50" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="K50" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="L50" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="M50">
         <v>0.1</v>
       </c>
       <c r="N50" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="O50">
         <v>0</v>
       </c>
-      <c r="Q50">
-        <v>0</v>
-      </c>
-      <c r="S50" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="51" spans="1:19" x14ac:dyDescent="0.4">
+      <c r="P50" t="s">
+        <v>87</v>
+      </c>
+      <c r="R50">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A51">
         <v>49</v>
       </c>
       <c r="B51" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C51">
         <v>20</v>
@@ -3393,51 +3392,51 @@
         <v>20</v>
       </c>
       <c r="E51" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F51" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="G51" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="H51" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="I51" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="J51" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="K51" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="L51" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="M51">
         <v>0.2</v>
       </c>
       <c r="N51" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="O51">
         <v>0</v>
       </c>
-      <c r="Q51">
-        <v>0</v>
-      </c>
-      <c r="S51" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="52" spans="1:19" x14ac:dyDescent="0.4">
+      <c r="P51" t="s">
+        <v>88</v>
+      </c>
+      <c r="R51">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A52">
         <v>50</v>
       </c>
       <c r="B52" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C52">
         <v>20</v>
@@ -3446,51 +3445,51 @@
         <v>20</v>
       </c>
       <c r="E52" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F52" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="G52" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="H52" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="I52" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="J52" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="K52" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="L52" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="M52">
         <v>0.5</v>
       </c>
       <c r="N52" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="O52">
         <v>0</v>
       </c>
-      <c r="Q52">
-        <v>0</v>
-      </c>
-      <c r="S52" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="53" spans="1:19" x14ac:dyDescent="0.4">
+      <c r="P52" t="s">
+        <v>89</v>
+      </c>
+      <c r="R52">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A53">
         <v>51</v>
       </c>
       <c r="B53" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C53">
         <v>20</v>
@@ -3499,51 +3498,51 @@
         <v>20</v>
       </c>
       <c r="E53" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F53" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="G53" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="H53" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="I53" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="J53" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="K53" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="L53" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="M53">
         <v>0.1</v>
       </c>
       <c r="N53" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="O53">
         <v>0</v>
       </c>
-      <c r="Q53">
-        <v>0</v>
-      </c>
-      <c r="S53" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="54" spans="1:19" x14ac:dyDescent="0.4">
+      <c r="P53" t="s">
+        <v>91</v>
+      </c>
+      <c r="R53">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A54">
         <v>52</v>
       </c>
       <c r="B54" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C54">
         <v>20</v>
@@ -3552,51 +3551,51 @@
         <v>20</v>
       </c>
       <c r="E54" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F54" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="G54" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="H54" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="I54" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="J54" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="K54" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="L54" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="M54">
         <v>0.2</v>
       </c>
       <c r="N54" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="O54">
         <v>0</v>
       </c>
-      <c r="Q54">
-        <v>0</v>
-      </c>
-      <c r="S54" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="55" spans="1:19" x14ac:dyDescent="0.4">
+      <c r="P54" t="s">
+        <v>92</v>
+      </c>
+      <c r="R54">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A55">
         <v>53</v>
       </c>
       <c r="B55" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C55">
         <v>20</v>
@@ -3605,51 +3604,51 @@
         <v>20</v>
       </c>
       <c r="E55" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F55" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="G55" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="H55" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="I55" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="J55" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="K55" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="L55" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="M55">
         <v>0.5</v>
       </c>
       <c r="N55" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="O55">
         <v>0</v>
       </c>
-      <c r="Q55">
-        <v>0</v>
-      </c>
-      <c r="S55" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="56" spans="1:19" x14ac:dyDescent="0.4">
+      <c r="P55" t="s">
+        <v>93</v>
+      </c>
+      <c r="R55">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A56">
         <v>54</v>
       </c>
       <c r="B56" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C56">
         <v>20</v>
@@ -3658,51 +3657,51 @@
         <v>20</v>
       </c>
       <c r="E56" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F56" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="G56" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="H56" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="I56" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="J56" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="K56" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="L56" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="M56">
         <v>0.1</v>
       </c>
       <c r="N56" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="O56">
         <v>0</v>
       </c>
-      <c r="Q56">
-        <v>0</v>
-      </c>
-      <c r="S56" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="57" spans="1:19" x14ac:dyDescent="0.4">
+      <c r="P56" t="s">
+        <v>95</v>
+      </c>
+      <c r="R56">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A57">
         <v>55</v>
       </c>
       <c r="B57" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C57">
         <v>20</v>
@@ -3711,51 +3710,51 @@
         <v>20</v>
       </c>
       <c r="E57" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F57" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="G57" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="H57" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="I57" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="J57" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="K57" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="L57" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="M57">
         <v>0.2</v>
       </c>
       <c r="N57" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="O57">
         <v>0</v>
       </c>
-      <c r="Q57">
-        <v>0</v>
-      </c>
-      <c r="S57" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="58" spans="1:19" x14ac:dyDescent="0.4">
+      <c r="P57" t="s">
+        <v>96</v>
+      </c>
+      <c r="R57">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A58">
         <v>56</v>
       </c>
       <c r="B58" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C58">
         <v>20</v>
@@ -3764,51 +3763,51 @@
         <v>20</v>
       </c>
       <c r="E58" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F58" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="G58" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="H58" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="I58" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="J58" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="K58" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="L58" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="M58">
         <v>0.5</v>
       </c>
       <c r="N58" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="O58">
         <v>0</v>
       </c>
-      <c r="Q58">
-        <v>0</v>
-      </c>
-      <c r="S58" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="59" spans="1:19" x14ac:dyDescent="0.4">
+      <c r="P58" t="s">
+        <v>97</v>
+      </c>
+      <c r="R58">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A59">
         <v>57</v>
       </c>
       <c r="B59" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C59">
         <v>20</v>
@@ -3817,51 +3816,51 @@
         <v>20</v>
       </c>
       <c r="E59" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F59" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="G59" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="H59" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="I59" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="J59" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="K59" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="L59" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="M59">
         <v>0.1</v>
       </c>
       <c r="N59" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="O59">
         <v>0</v>
       </c>
-      <c r="Q59">
-        <v>0</v>
-      </c>
-      <c r="S59" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="60" spans="1:19" x14ac:dyDescent="0.4">
+      <c r="P59" t="s">
+        <v>99</v>
+      </c>
+      <c r="R59">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A60">
         <v>58</v>
       </c>
       <c r="B60" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C60">
         <v>20</v>
@@ -3870,51 +3869,51 @@
         <v>20</v>
       </c>
       <c r="E60" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F60" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="G60" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="H60" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="I60" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="J60" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="K60" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="L60" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="M60">
         <v>0.2</v>
       </c>
       <c r="N60" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="O60">
         <v>0</v>
       </c>
-      <c r="Q60">
-        <v>0</v>
-      </c>
-      <c r="S60" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="61" spans="1:19" x14ac:dyDescent="0.4">
+      <c r="P60" t="s">
+        <v>100</v>
+      </c>
+      <c r="R60">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A61">
         <v>59</v>
       </c>
       <c r="B61" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C61">
         <v>20</v>
@@ -3923,51 +3922,51 @@
         <v>20</v>
       </c>
       <c r="E61" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F61" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="G61" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="H61" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="I61" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="J61" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="K61" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="L61" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="M61">
         <v>0.5</v>
       </c>
       <c r="N61" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="O61">
         <v>0</v>
       </c>
-      <c r="Q61">
-        <v>0</v>
-      </c>
-      <c r="S61" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="62" spans="1:19" x14ac:dyDescent="0.4">
+      <c r="P61" t="s">
+        <v>101</v>
+      </c>
+      <c r="R61">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A62">
         <v>60</v>
       </c>
       <c r="B62" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C62">
         <v>20</v>
@@ -3976,43 +3975,43 @@
         <v>20</v>
       </c>
       <c r="E62" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F62" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="G62" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="H62" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="I62" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="J62" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="K62" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="L62" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="M62" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="N62" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="O62">
         <v>1</v>
       </c>
-      <c r="Q62">
-        <v>0</v>
-      </c>
-      <c r="S62" t="s">
-        <v>105</v>
+      <c r="P62" t="s">
+        <v>103</v>
+      </c>
+      <c r="R62">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>